<commit_message>
rename file and deleting note relevant for testing
</commit_message>
<xml_diff>
--- a/server/tests/files_to_test/students_list_excel/example_excel_start_in_random_row.xlsx
+++ b/server/tests/files_to_test/students_list_excel/example_excel_start_in_random_row.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inbar Shirizly\Documents\python\useful\ITC_programs\zoom_attendance_check\server\test\files_to_test\students_list_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inbar_Shirizly\Documents\python\useful\ITC_programs\zoom_attendance_check\server\tests\files_to_test\students_list_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C50AEC-96BE-457A-A752-9131305BC3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D446733B-85EE-4AC4-B029-07B9E9C71A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{488C6C20-8654-4E36-919F-D3E2AD714F5E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{488C6C20-8654-4E36-919F-D3E2AD714F5E}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>עידן אביב</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>id_number</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
 </sst>
 </file>
@@ -431,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949A20AF-119A-42AC-AEC9-B52646CBA3DA}">
-  <dimension ref="C2:I18"/>
+  <dimension ref="D2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,25 +444,22 @@
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
@@ -485,10 +479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12">
-        <v>11</v>
-      </c>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="2">
         <v>528702484</v>
       </c>
@@ -499,10 +490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C13">
-        <v>12</v>
-      </c>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13" s="3">
         <v>524291930</v>
       </c>
@@ -513,10 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14">
-        <v>13</v>
-      </c>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14">
         <v>526148959</v>
       </c>
@@ -527,10 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15">
-        <v>14</v>
-      </c>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>523454564</v>
       </c>
@@ -541,10 +523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16">
-        <v>15</v>
-      </c>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>530342423</v>
       </c>
@@ -555,10 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17">
-        <v>16</v>
-      </c>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17">
         <v>530342413</v>
       </c>
@@ -569,10 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <v>17</v>
-      </c>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>537642324</v>
       </c>

</xml_diff>